<commit_message>
freebayes 10 and 17 parallel
</commit_message>
<xml_diff>
--- a/shells/Freebayes/analysis_log.xlsx
+++ b/shells/Freebayes/analysis_log.xlsx
@@ -341,13 +341,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -631,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,16 +712,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>168460001</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>134208390</v>
       </c>
       <c r="E4">

</xml_diff>